<commit_message>
feat: sops Update 3
</commit_message>
<xml_diff>
--- a/5-Software Service Catalog -SS/Forms/Release Form - F5.xlsx
+++ b/5-Software Service Catalog -SS/Forms/Release Form - F5.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heba.backar\Downloads\SW 2025 2\SW 2025\SW 2025\1-Software Development Lifecycle\Forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QMS\5-Software Service Catalog -SS\Forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D01503-DAB5-4A1D-A0D7-776630DCFA74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCBBC105-0ADE-4C13-846C-7910AE27BABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AFD02EE8-0092-4247-AD75-3F54CC0C98CB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10245" windowHeight="10920" xr2:uid="{AFD02EE8-0092-4247-AD75-3F54CC0C98CB}"/>
   </bookViews>
   <sheets>
-    <sheet name="F-SW-SD-05" sheetId="1" r:id="rId1"/>
+    <sheet name="S-SW-SC-05" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'F-SW-SD-05'!$A$1:$E$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'S-SW-SC-05'!$A$1:$E$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -219,6 +219,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -229,9 +247,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -241,15 +256,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -269,12 +275,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -688,121 +688,116 @@
     <row r="1" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="27"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="21"/>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="19"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="19"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="14"/>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="19"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="14"/>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="19"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="14"/>
       <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="27"/>
       <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="22"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="24"/>
       <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="11"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="11"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A11:E11"/>
     <mergeCell ref="A12:E12"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A7:B7"/>
@@ -816,6 +811,11 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="C9:E9"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A11:E11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>